<commit_message>
added smoke test testng.xml file
</commit_message>
<xml_diff>
--- a/src/main/resources/SwagLabTestData.xlsx
+++ b/src/main/resources/SwagLabTestData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohit_panwar\eclipse-workspace\SeleniumFrameWorkUsingJava\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F5FCC1-3F08-4248-A9D5-83F9E16CC3E3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B65A8A2-8ACF-49B0-879C-5BE58176FFCD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{5115D751-2ED6-4C43-922B-770A75FFD0DE}"/>
   </bookViews>
   <sheets>
     <sheet name="UserList" sheetId="1" r:id="rId1"/>
     <sheet name="Sorting" sheetId="2" r:id="rId2"/>
+    <sheet name="UserList (2)" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
     <t>UserName</t>
   </si>
@@ -79,10 +80,10 @@
     <t>Sauce Labs Fleece Jacket</t>
   </si>
   <si>
-    <t>Sauce Labs OnesieM</t>
-  </si>
-  <si>
-    <t>Sauce Labs BackpackM</t>
+    <t>Sauce Labs Onesie</t>
+  </si>
+  <si>
+    <t>Sauce Labs Backpack</t>
   </si>
 </sst>
 </file>
@@ -468,7 +469,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B5"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,7 +529,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,4 +582,56 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BAF5210-654A-4A7B-A44F-843A097F2D28}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>